<commit_message>
solved the issue when reading double value from excel.
</commit_message>
<xml_diff>
--- a/OfficeTests/TestData/ManualCreated.xlsx
+++ b/OfficeTests/TestData/ManualCreated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fengy\CodeProjects\Personal\DotNetCommonLib\OfficeTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D643B5-6738-434B-A3C7-D0E790A4B8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2C442F-C949-4409-9785-4FE75CE874D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="3040" windowWidth="23040" windowHeight="13570" xr2:uid="{D67B7A2E-730C-4F7A-9BCA-FB534A85CA74}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Number" sheetId="3" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Text" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>adsfsdf</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -173,6 +174,30 @@
   </si>
   <si>
     <t>3000.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.332</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigvalue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200000000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -236,7 +261,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -280,6 +305,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FACC598-197A-4049-93CA-8A06AD2F2EE6}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -704,9 +732,44 @@
         <v>33</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <f xml:space="preserve"> 0.1 + 0.2</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>200000000000</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -937,4 +1000,17 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48ED18B-5A68-413A-9310-4E8DA338EE1C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>